<commit_message>
Corrijo modelo y agrego mejoras para compatibilidad en streamlit cloud
</commit_message>
<xml_diff>
--- a/estadisticas_equipos.xlsx
+++ b/estadisticas_equipos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ander\Desktop\PrediccionPartidosFutbol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19709EE6-0685-4097-83C8-CE68ED19F752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67988C25-77C9-4CBB-A859-5A1CCF67A599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{77B7C34B-EF32-4F32-A033-12C1BE94881A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Equipo</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Esquina</t>
+  </si>
+  <si>
+    <t>Psg</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56365DE4-B83C-40EC-B059-4AE26BCAAAB0}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,13 +487,13 @@
         <v>39</v>
       </c>
       <c r="H2">
-        <v>23</v>
+        <v>676</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="J2">
-        <v>10</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -516,13 +519,45 @@
         <v>38</v>
       </c>
       <c r="H3">
-        <v>9</v>
+        <v>634</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="J3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
         <v>2</v>
+      </c>
+      <c r="F4">
+        <v>92</v>
+      </c>
+      <c r="G4">
+        <v>35</v>
+      </c>
+      <c r="H4">
+        <v>636</v>
+      </c>
+      <c r="I4">
+        <v>41</v>
+      </c>
+      <c r="J4">
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>